<commit_message>
[update]: individual parts of paper is updated
</commit_message>
<xml_diff>
--- a/CURRENT WORK/SALT WORK - CODES/N = 3/Li2SO4 - Done/Test_excelsheet for Li2SO4 n=3.xlsx
+++ b/CURRENT WORK/SALT WORK - CODES/N = 3/Li2SO4 - Done/Test_excelsheet for Li2SO4 n=3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhanu\OneDrive\Desktop\FYP\Current Work\SALT WORK\N = 3\Li2SO4 - Done\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dhanu\OneDrive\Desktop\Final-Year-Project\CURRENT WORK\SALT WORK - CODES\N = 3\Li2SO4 - Done\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6B847B-1273-458D-B3ED-4A4F69F2F0DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C91C5FB-0C68-4691-AB5C-1660F30DC475}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="696" activeTab="4" xr2:uid="{86974002-CAD5-4FCC-AF77-EBAA345E04BF}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="696" firstSheet="1" activeTab="1" xr2:uid="{86974002-CAD5-4FCC-AF77-EBAA345E04BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Exp - Osmotic Coefficient" sheetId="1" r:id="rId1"/>
@@ -644,22 +644,46 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1320" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-IN"/>
-              <a:t>Parity Plot for Li2SO4 for n=3</a:t>
+              <a:t>Fig 8. Parity Plot for Li</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IN" sz="900"/>
+              <a:t>2</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IN"/>
+              <a:t>SO</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IN" sz="900"/>
+              <a:t>4</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IN"/>
+              <a:t> for n=3</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.27708480613147596"/>
+          <c:y val="0.92152030469692914"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -673,11 +697,11 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1320" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx2"/>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -688,7 +712,17 @@
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.13825412093749154"/>
+          <c:y val="9.628249510360129E-2"/>
+          <c:w val="0.82035069013872308"/>
+          <c:h val="0.66184596038072663"/>
+        </c:manualLayout>
+      </c:layout>
       <c:scatterChart>
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
@@ -1020,11 +1054,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
@@ -1049,11 +1083,11 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx2"/>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
@@ -1080,11 +1114,11 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -1112,11 +1146,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
@@ -1141,11 +1175,11 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx2"/>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
@@ -1172,11 +1206,11 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -1229,7 +1263,12 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -4661,34 +4700,46 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1320" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
               <a:rPr lang="en-IN"/>
-              <a:t>Temperature vs </a:t>
+              <a:t>Fig 7. Temperature vs Ø for Li</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-IN">
-                <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-              </a:rPr>
-              <a:t>Ø</a:t>
+              <a:rPr lang="en-IN" sz="900"/>
+              <a:t>2</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-IN"/>
-              <a:t> for Li2SO4 n=3</a:t>
+              <a:t>SO</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IN" sz="900"/>
+              <a:t>4</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-IN"/>
+              <a:t> n=3</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.20786319444444445"/>
+          <c:y val="0.89664351851851842"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -4702,11 +4753,11 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1320" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx2"/>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
+              <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -6325,24 +6376,19 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-IN" sz="1400">
-                    <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                    <a:ea typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                    <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
-                  </a:rPr>
+                  <a:rPr lang="en-IN"/>
                   <a:t>Ø</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-IN" sz="1400"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -6359,11 +6405,11 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx2"/>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
@@ -6391,11 +6437,11 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -6406,6 +6452,7 @@
         <c:crossAx val="472873184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="4.0000000000000008E-2"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="472873184"/>
@@ -6421,11 +6468,11 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx2"/>
+                      <a:sysClr val="windowText" lastClr="000000"/>
                     </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
+                    <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
@@ -6450,11 +6497,11 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1100" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
-                    <a:schemeClr val="tx2"/>
+                    <a:sysClr val="windowText" lastClr="000000"/>
                   </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
+                  <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
@@ -6481,11 +6528,11 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx2"/>
+                  <a:sysClr val="windowText" lastClr="000000"/>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
@@ -6513,10 +6560,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.13941059870993175"/>
-          <c:y val="0.17413127729481273"/>
-          <c:w val="0.26916193021074031"/>
-          <c:h val="0.14602134150504861"/>
+          <c:x val="0.1688087962962963"/>
+          <c:y val="0.11239513888888888"/>
+          <c:w val="0.37205555555555553"/>
+          <c:h val="0.15778055555555556"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -6534,11 +6581,11 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx2"/>
+                <a:sysClr val="windowText" lastClr="000000"/>
               </a:solidFill>
-              <a:latin typeface="Abadi" panose="020B0604020104020204" pitchFamily="34" charset="0"/>
+              <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
@@ -6578,7 +6625,12 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1100">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:latin typeface="Palatino Linotype" panose="02040502050505030304" pitchFamily="18" charset="0"/>
+        </a:defRPr>
       </a:pPr>
       <a:endParaRPr lang="en-US"/>
     </a:p>
@@ -10593,13 +10645,13 @@
       <xdr:col>47</xdr:col>
       <xdr:colOff>194880</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>46025</xdr:rowOff>
+      <xdr:rowOff>46024</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>55</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>54</xdr:col>
+      <xdr:colOff>247680</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>167404</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -10633,12 +10685,12 @@
 <c:userShapes xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.10891</cdr:x>
-      <cdr:y>0.1453</cdr:y>
+      <cdr:x>0.1401</cdr:x>
+      <cdr:y>0.09768</cdr:y>
     </cdr:from>
     <cdr:to>
       <cdr:x>0.95879</cdr:x>
-      <cdr:y>0.85149</cdr:y>
+      <cdr:y>0.75664</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
@@ -10653,8 +10705,8 @@
       </cdr:nvCxnSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" flipV="1">
-          <a:off x="563851" y="502615"/>
-          <a:ext cx="4400009" cy="2442838"/>
+          <a:off x="605220" y="421956"/>
+          <a:ext cx="3536753" cy="2846720"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
           <a:avLst/>
@@ -10679,12 +10731,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.1319</cdr:x>
-      <cdr:y>0.14907</cdr:y>
+      <cdr:x>0.13719</cdr:x>
+      <cdr:y>0.09615</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.39949</cdr:x>
-      <cdr:y>0.25544</cdr:y>
+      <cdr:x>0.43819</cdr:x>
+      <cdr:y>0.19749</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -10699,8 +10751,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="682868" y="515646"/>
-          <a:ext cx="1385392" cy="367969"/>
+          <a:off x="592668" y="415382"/>
+          <a:ext cx="1300332" cy="437754"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect">
           <a:avLst/>
@@ -10852,12 +10904,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.1702</cdr:x>
-      <cdr:y>0.17397</cdr:y>
+      <cdr:x>0.17726</cdr:x>
+      <cdr:y>0.11576</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.18755</cdr:x>
-      <cdr:y>0.19596</cdr:y>
+      <cdr:x>0.19461</cdr:x>
+      <cdr:y>0.13775</cdr:y>
     </cdr:to>
     <cdr:sp macro="" textlink="">
       <cdr:nvSpPr>
@@ -10872,8 +10924,8 @@
       </cdr:nvSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="881155" y="601790"/>
-          <a:ext cx="89826" cy="76085"/>
+          <a:off x="765744" y="500090"/>
+          <a:ext cx="74952" cy="94997"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="flowChartConnector">
           <a:avLst/>
@@ -11001,12 +11053,12 @@
   </cdr:relSizeAnchor>
   <cdr:relSizeAnchor xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing">
     <cdr:from>
-      <cdr:x>0.15733</cdr:x>
-      <cdr:y>0.23045</cdr:y>
+      <cdr:x>0.16791</cdr:x>
+      <cdr:y>0.16519</cdr:y>
     </cdr:from>
     <cdr:to>
-      <cdr:x>0.20421</cdr:x>
-      <cdr:y>0.23045</cdr:y>
+      <cdr:x>0.21479</cdr:x>
+      <cdr:y>0.16519</cdr:y>
     </cdr:to>
     <cdr:cxnSp macro="">
       <cdr:nvCxnSpPr>
@@ -11021,8 +11073,8 @@
       </cdr:nvCxnSpPr>
       <cdr:spPr>
         <a:xfrm xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-          <a:off x="814518" y="797172"/>
-          <a:ext cx="242719" cy="0"/>
+          <a:off x="725386" y="713604"/>
+          <a:ext cx="202521" cy="0"/>
         </a:xfrm>
         <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="line">
           <a:avLst/>
@@ -11211,10 +11263,10 @@
       <xdr:rowOff>179070</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>220980</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>22860</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>68040</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>109950</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12613,8 +12665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88D00978-96AD-440F-AA3F-9C948C561128}">
   <dimension ref="A1:AU84"/>
   <sheetViews>
-    <sheetView topLeftCell="AP6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="BG20" sqref="BG20"/>
+    <sheetView tabSelected="1" topLeftCell="AP7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="BD22" sqref="BD22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -24162,8 +24214,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAA53125-8324-42F8-BF4C-83E8BB87300B}">
   <dimension ref="A1:E219"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26336,20 +26388,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="49fa8af8-517d-491f-a3d5-7cf68fb985f9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="49fa8af8-517d-491f-a3d5-7cf68fb985f9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -26372,6 +26424,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71225005-2353-48CA-B97F-AA326ECE473F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{715EA469-2506-458C-8899-792543708004}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -26386,12 +26446,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71225005-2353-48CA-B97F-AA326ECE473F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
few reference files added
</commit_message>
<xml_diff>
--- a/CURRENT WORK/SALT WORK - CODES/N = 3/Li2SO4 - Done/Test_excelsheet for Li2SO4 n=3.xlsx
+++ b/CURRENT WORK/SALT WORK - CODES/N = 3/Li2SO4 - Done/Test_excelsheet for Li2SO4 n=3.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{6A685E10-A004-4175-9CB8-7A5AFC20C99B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58B4B991-E4CD-4C35-A227-DF91151E6132}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="696" firstSheet="1" activeTab="1" xr2:uid="{86974002-CAD5-4FCC-AF77-EBAA345E04BF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" tabRatio="696" xr2:uid="{86974002-CAD5-4FCC-AF77-EBAA345E04BF}"/>
   </bookViews>
   <sheets>
     <sheet name="Exp - Osmotic Coefficient" sheetId="1" r:id="rId1"/>
@@ -11447,7 +11447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FE59662-707B-4A33-B0E4-F8A5EA30B87F}">
   <dimension ref="A1:K69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -12345,7 +12345,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88D00978-96AD-440F-AA3F-9C948C561128}">
   <dimension ref="A1:AX84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AQ10" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="AQ1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="BK13" sqref="BK13"/>
     </sheetView>
   </sheetViews>
@@ -26231,20 +26231,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="49fa8af8-517d-491f-a3d5-7cf68fb985f9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="49fa8af8-517d-491f-a3d5-7cf68fb985f9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -26267,14 +26267,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71225005-2353-48CA-B97F-AA326ECE473F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{715EA469-2506-458C-8899-792543708004}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -26289,4 +26281,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71225005-2353-48CA-B97F-AA326ECE473F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>